<commit_message>
Terem kihasználtság funkció fejlesztése
</commit_message>
<xml_diff>
--- a/NAPI_MENTÉS_2018_JÚNIUS.xlsx
+++ b/NAPI_MENTÉS_2018_JÚNIUS.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gábor_1\Documents\Programozás\Java_projects\draw_to_console\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABF81B3-AABC-4F8C-96D0-8CE2E4580219}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="21075" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="NAPI_MENTÉS_2018_JÚNIUS" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="10">
   <si>
     <t>JÁVOR PÁL TEREM</t>
   </si>
@@ -54,56 +48,31 @@
   <si>
     <t>BLADE RUNNER 3D</t>
   </si>
-  <si>
-    <t>Dátum</t>
-  </si>
-  <si>
-    <t>Terem</t>
-  </si>
-  <si>
-    <t>Teremnév</t>
-  </si>
-  <si>
-    <t>Film</t>
-  </si>
-  <si>
-    <t>FilmCím</t>
-  </si>
-  <si>
-    <t>Foglalt</t>
-  </si>
-  <si>
-    <t>Szabad</t>
-  </si>
-  <si>
-    <t>Jegyár</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="238"/>
       <scheme val="major"/>
@@ -112,129 +81,114 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -556,74 +510,74 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 2. jelölőszín" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 3. jelölőszín" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 4. jelölőszín" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 5. jelölőszín" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 6. jelölőszín" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 1. jelölőszín" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 2. jelölőszín" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 3. jelölőszín" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 4. jelölőszín" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 5. jelölőszín" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 6. jelölőszín" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 1. jelölőszín" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 2. jelölőszín" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 3. jelölőszín" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 4. jelölőszín" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 5. jelölőszín" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 6. jelölőszín" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bevitel" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Cím" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Címsor 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Címsor 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Címsor 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Címsor 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Ellenőrzőcella" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Figyelmeztetés" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Hivatkozott cella" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Jegyzet" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Jelölőszín 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Jó" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kimenet" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Magyarázó szöveg" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
-    <cellStyle name="Összesen" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Rossz" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Semleges" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Számítás" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,15 +585,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -649,44 +600,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -714,31 +665,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -766,23 +700,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -794,183 +711,184 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="8" width="30.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20180626</v>
       </c>
@@ -996,7 +914,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20180626</v>
       </c>
@@ -1022,7 +940,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20180626</v>
       </c>
@@ -1048,7 +966,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20180626</v>
       </c>
@@ -1065,16 +983,16 @@
         <v>7</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G5">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>990</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20180626</v>
       </c>
@@ -1100,7 +1018,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20180626</v>
       </c>
@@ -1126,7 +1044,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20180626</v>
       </c>
@@ -1152,7 +1070,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20180626</v>
       </c>
@@ -1178,7 +1096,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20180626</v>
       </c>
@@ -1195,16 +1113,16 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="G10">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>990</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20180626</v>
       </c>
@@ -1230,7 +1148,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20180626</v>
       </c>
@@ -1256,7 +1174,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20180626</v>
       </c>
@@ -1282,7 +1200,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20180626</v>
       </c>
@@ -1308,7 +1226,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20180626</v>
       </c>
@@ -1325,16 +1243,16 @@
         <v>7</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G15">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>990</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20180626</v>
       </c>
@@ -1360,7 +1278,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20180626</v>
       </c>
@@ -1386,7 +1304,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20180626</v>
       </c>
@@ -1412,7 +1330,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20180626</v>
       </c>
@@ -1438,7 +1356,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20180626</v>
       </c>
@@ -1455,16 +1373,16 @@
         <v>7</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G20">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>990</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20180626</v>
       </c>
@@ -1490,7 +1408,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20180626</v>
       </c>
@@ -1516,7 +1434,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20180626</v>
       </c>
@@ -1542,7 +1460,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20180626</v>
       </c>
@@ -1568,7 +1486,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20180626</v>
       </c>
@@ -1585,16 +1503,16 @@
         <v>7</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G25">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>990</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20180626</v>
       </c>
@@ -1620,7 +1538,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20180626</v>
       </c>
@@ -1637,16 +1555,16 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="G27">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>1990</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20180626</v>
       </c>
@@ -1672,7 +1590,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20180626</v>
       </c>
@@ -1698,7 +1616,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20180626</v>
       </c>
@@ -1715,16 +1633,16 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G30">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>990</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20180626</v>
       </c>
@@ -1750,7 +1668,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20180628</v>
       </c>
@@ -1776,7 +1694,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20180628</v>
       </c>
@@ -1802,7 +1720,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20180628</v>
       </c>
@@ -1828,7 +1746,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20180628</v>
       </c>
@@ -1845,16 +1763,16 @@
         <v>7</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G35">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>990</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20180628</v>
       </c>
@@ -1881,7 +1799,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:H36">
     <filterColumn colId="1">
       <filters>
         <filter val="8"/>

</xml_diff>

<commit_message>
Statisztikák főmenü almenüiben lévő funkciók elkészítése, kisebb
hibajavítások a programban végig, tesztelés.
</commit_message>
<xml_diff>
--- a/NAPI_MENTÉS_2018_JÚNIUS.xlsx
+++ b/NAPI_MENTÉS_2018_JÚNIUS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gábor_1\Documents\Programozás\Java_projects\draw_to_console\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0A8601-D0D4-4718-9DFA-687CEAE375AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="21075" windowHeight="11835"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="21072" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAPI_MENTÉS_2018_JÚNIUS" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NAPI_MENTÉS_2018_JÚNIUS!$A$1:$H$36</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -52,7 +58,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -488,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -531,53 +541,57 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 2. jelölőszín" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 3. jelölőszín" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 4. jelölőszín" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 5. jelölőszín" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 6. jelölőszín" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 1. jelölőszín" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 2. jelölőszín" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 3. jelölőszín" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 4. jelölőszín" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 5. jelölőszín" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 6. jelölőszín" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 1. jelölőszín" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 2. jelölőszín" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 3. jelölőszín" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 4. jelölőszín" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 5. jelölőszín" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 6. jelölőszín" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bevitel" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Cím" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Címsor 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Címsor 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Címsor 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Címsor 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Ellenőrzőcella" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Figyelmeztetés" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Hivatkozott cella" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Jegyzet" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Jelölőszín 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Jó" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kimenet" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Magyarázó szöveg" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Összesen" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Pénznem" xfId="42" builtinId="4"/>
+    <cellStyle name="Rossz" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Semleges" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Számítás" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -585,12 +599,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -632,7 +649,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,9 +682,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,6 +734,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -875,20 +926,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:H36"/>
+  <dimension ref="A2:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="I5" sqref="I5:I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="30.42578125" customWidth="1"/>
+    <col min="1" max="5" width="30.44140625" customWidth="1"/>
+    <col min="6" max="7" width="30.44140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180626</v>
       </c>
@@ -904,17 +958,21 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>145</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="1">
+        <f>F2*H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180626</v>
       </c>
@@ -930,17 +988,21 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>230</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I36" si="0">F3*H3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180626</v>
       </c>
@@ -956,17 +1018,21 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20180626</v>
       </c>
@@ -982,17 +1048,21 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>80</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20180626</v>
       </c>
@@ -1008,17 +1078,21 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>54</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20180626</v>
       </c>
@@ -1034,17 +1108,21 @@
       <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>135</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>19900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20180626</v>
       </c>
@@ -1060,17 +1138,21 @@
       <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>20</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>210</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>29800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20180626</v>
       </c>
@@ -1086,17 +1168,21 @@
       <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>28</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>72</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>41720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20180626</v>
       </c>
@@ -1112,17 +1198,21 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>80</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20180626</v>
       </c>
@@ -1138,17 +1228,21 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>32</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>22</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>76480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20180626</v>
       </c>
@@ -1164,17 +1258,21 @@
       <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
         <v>145</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20180626</v>
       </c>
@@ -1190,17 +1288,21 @@
       <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
         <v>230</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20180626</v>
       </c>
@@ -1216,17 +1318,21 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
         <v>100</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20180626</v>
       </c>
@@ -1242,17 +1348,21 @@
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>80</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20180626</v>
       </c>
@@ -1268,17 +1378,21 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
         <v>54</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20180626</v>
       </c>
@@ -1294,17 +1408,21 @@
       <c r="E17" t="s">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
         <v>145</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20180626</v>
       </c>
@@ -1320,17 +1438,21 @@
       <c r="E18" t="s">
         <v>3</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
         <v>230</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20180626</v>
       </c>
@@ -1346,17 +1468,21 @@
       <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
         <v>100</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20180626</v>
       </c>
@@ -1372,17 +1498,21 @@
       <c r="E20" t="s">
         <v>7</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>80</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20180626</v>
       </c>
@@ -1398,17 +1528,21 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
         <v>54</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20180626</v>
       </c>
@@ -1424,17 +1558,21 @@
       <c r="E22" t="s">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
         <v>145</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20180626</v>
       </c>
@@ -1450,17 +1588,21 @@
       <c r="E23" t="s">
         <v>3</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
         <v>230</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20180626</v>
       </c>
@@ -1476,17 +1618,21 @@
       <c r="E24" t="s">
         <v>5</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
         <v>100</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20180626</v>
       </c>
@@ -1502,17 +1648,21 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>80</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20180626</v>
       </c>
@@ -1528,17 +1678,21 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
         <v>54</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20180626</v>
       </c>
@@ -1554,17 +1708,21 @@
       <c r="E27" t="s">
         <v>1</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>145</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>288550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20180626</v>
       </c>
@@ -1580,17 +1738,21 @@
       <c r="E28" t="s">
         <v>3</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
         <v>230</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20180626</v>
       </c>
@@ -1606,17 +1768,21 @@
       <c r="E29" t="s">
         <v>5</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
         <v>100</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20180626</v>
       </c>
@@ -1632,17 +1798,21 @@
       <c r="E30" t="s">
         <v>7</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>80</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20180626</v>
       </c>
@@ -1658,17 +1828,21 @@
       <c r="E31" t="s">
         <v>9</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
         <v>54</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1">
         <v>2390</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20180628</v>
       </c>
@@ -1684,17 +1858,21 @@
       <c r="E32" t="s">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
         <v>145</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>1990</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20180628</v>
       </c>
@@ -1710,17 +1888,21 @@
       <c r="E33" t="s">
         <v>3</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
         <v>230</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20180628</v>
       </c>
@@ -1736,17 +1918,21 @@
       <c r="E34" t="s">
         <v>5</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
         <v>100</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20180628</v>
       </c>
@@ -1762,17 +1948,21 @@
       <c r="E35" t="s">
         <v>7</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>80</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
         <v>990</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>79200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20180628</v>
       </c>
@@ -1788,21 +1978,25 @@
       <c r="E36" t="s">
         <v>9</v>
       </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
         <v>54</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>2390</v>
       </c>
+      <c r="I36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H36">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="4">
       <filters>
-        <filter val="8"/>
+        <filter val="BLADE RUNNER 3D"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>